<commit_message>
Changed database structure document to reflect changes
</commit_message>
<xml_diff>
--- a/DatabaseStructure.xlsx
+++ b/DatabaseStructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\GitHub\OOSD2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Sprackle\Documents\GitHub\OOSD2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{987B7364-FE0B-41AF-B21B-9CB031C56C00}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" xr2:uid="{987B7364-FE0B-41AF-B21B-9CB031C56C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>Users</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>HallRooms</t>
-  </si>
-  <si>
     <t>HallUID</t>
   </si>
   <si>
@@ -110,13 +107,13 @@
     <t>string</t>
   </si>
   <si>
-    <t>RoomLeases</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>LeaseUID</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -140,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -286,11 +283,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -306,6 +344,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,116 +673,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B633A115-10B1-4995-9841-ED9C938BEB70}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -738,107 +791,119 @@
         <v>6</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
       <c r="I7" s="7"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
@@ -849,54 +914,50 @@
       <c r="I8" s="8"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>26</v>
-      </c>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>